<commit_message>
se añaden listas de simbolos no terminales
</commit_message>
<xml_diff>
--- a/recursos/matriz_sintactica.xlsx
+++ b/recursos/matriz_sintactica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Kevin Barboza\Documents\Kevin\10mo semestre\compiladores\proyecto_compilador\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D93588-4569-46CD-8552-D61AB137A1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFF6C02-C63E-406D-8410-58786B78AE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E76F90DD-ACB3-4C38-8BB9-83327DEBFBE5}"/>
   </bookViews>
@@ -33,6 +33,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -783,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA0880F-1227-4CE0-8563-1A06A3D886E6}">
-  <dimension ref="A1:BJ44"/>
+  <dimension ref="A1:BJ46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC18" sqref="AC18"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9071,6 +9093,138 @@
         <v>92</v>
       </c>
     </row>
+    <row r="46" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="str" cm="1">
+        <f t="array" ref="A46:AQ46">TRANSPOSE(A2:A44)</f>
+        <v>PROGRAMA</v>
+      </c>
+      <c r="B46" s="6" t="str">
+        <v>DECLARACIONVARIABLES</v>
+      </c>
+      <c r="C46" s="6" t="str">
+        <v>VARIABLES</v>
+      </c>
+      <c r="D46" s="6" t="str">
+        <v>LISTAVARIABLES</v>
+      </c>
+      <c r="E46" s="6" t="str">
+        <v>LISTAVARIABLESPRIMA</v>
+      </c>
+      <c r="F46" s="6" t="str">
+        <v>TIPO</v>
+      </c>
+      <c r="G46" s="6" t="str">
+        <v>FUNCIONES</v>
+      </c>
+      <c r="H46" s="6" t="str">
+        <v>FUNCION</v>
+      </c>
+      <c r="I46" s="6" t="str">
+        <v>MAIN</v>
+      </c>
+      <c r="J46" s="6" t="str">
+        <v>PARAMETROS</v>
+      </c>
+      <c r="K46" s="6" t="str">
+        <v>RETURN</v>
+      </c>
+      <c r="L46" s="6" t="str">
+        <v>LISTARETURN</v>
+      </c>
+      <c r="M46" s="6" t="str">
+        <v>LISTARETURNPRIMA</v>
+      </c>
+      <c r="N46" s="6" t="str">
+        <v>BLOQUE</v>
+      </c>
+      <c r="O46" s="6" t="str">
+        <v>ESTATUTOS</v>
+      </c>
+      <c r="P46" s="6" t="str">
+        <v>ESTATUTO</v>
+      </c>
+      <c r="Q46" s="6" t="str">
+        <v>LISTA</v>
+      </c>
+      <c r="R46" s="6" t="str">
+        <v>LISTAELEMENTOS</v>
+      </c>
+      <c r="S46" s="6" t="str">
+        <v>LISTAPRIMA</v>
+      </c>
+      <c r="T46" s="6" t="str">
+        <v>ELEMENTO_TEXTOSPRIMA</v>
+      </c>
+      <c r="U46" s="6" t="str">
+        <v>ELEMENTO_NUMEROSPRIMA</v>
+      </c>
+      <c r="V46" s="6" t="str">
+        <v>FUNCION_BUILT_IN</v>
+      </c>
+      <c r="W46" s="6" t="str">
+        <v>VARIABLESIMPRIMIR</v>
+      </c>
+      <c r="X46" s="6" t="str">
+        <v>VARIABLESPRIMA</v>
+      </c>
+      <c r="Y46" s="6" t="str">
+        <v>ELSEIF</v>
+      </c>
+      <c r="Z46" s="6" t="str">
+        <v>ELSE</v>
+      </c>
+      <c r="AA46" s="6" t="str">
+        <v>RANGO</v>
+      </c>
+      <c r="AB46" s="6" t="str">
+        <v>VALOR1</v>
+      </c>
+      <c r="AC46" s="6" t="str">
+        <v>VALOR2</v>
+      </c>
+      <c r="AD46" s="6" t="str">
+        <v>VALOR3</v>
+      </c>
+      <c r="AE46" s="6" t="str">
+        <v>BOOLEXP</v>
+      </c>
+      <c r="AF46" s="6" t="str">
+        <v>BOOLEXP_PRIMA</v>
+      </c>
+      <c r="AG46" s="6" t="str">
+        <v>BOOLTERM</v>
+      </c>
+      <c r="AH46" s="6" t="str">
+        <v>BOOLTERM_PRIMA</v>
+      </c>
+      <c r="AI46" s="6" t="str">
+        <v>BOOLFACTOR</v>
+      </c>
+      <c r="AJ46" s="6" t="str">
+        <v>RELTERMP</v>
+      </c>
+      <c r="AK46" s="6" t="str">
+        <v>RELTERM</v>
+      </c>
+      <c r="AL46" s="6" t="str">
+        <v>EXPARITM</v>
+      </c>
+      <c r="AM46" s="6" t="str">
+        <v>EXPPRIMA</v>
+      </c>
+      <c r="AN46" s="6" t="str">
+        <v>TERMINO</v>
+      </c>
+      <c r="AO46" s="6" t="str">
+        <v>TERMPRIMO</v>
+      </c>
+      <c r="AP46" s="6" t="str">
+        <v>FACTOR</v>
+      </c>
+      <c r="AQ46" s="6" t="str">
+        <v>OPERADOR</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="BD18:BJ18 BD23:BJ23 AB18:BB18 AB2:BJ17 AB24:BJ36 AB23:BB23 AB20:BJ22 B37:BJ44 B2:AA18 B20:AA36 B19:BJ19">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">

</xml_diff>